<commit_message>
fix: started code refactoring
</commit_message>
<xml_diff>
--- a/firmware/Code/Bicopter_MPU/config_data.xlsx
+++ b/firmware/Code/Bicopter_MPU/config_data.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\Github\Horizon\firmware\Code\Bicopter_MPU\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{289E0CFF-E7CB-456C-B3F3-910E22C66213}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{691E5DF0-0280-4AD7-8597-95E81C5E58D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="0" windowWidth="14400" windowHeight="8100" activeTab="2" xr2:uid="{2840FDD2-01AF-4896-868F-3F8C8BCC030E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{2840FDD2-01AF-4896-868F-3F8C8BCC030E}"/>
   </bookViews>
   <sheets>
     <sheet name="Pinout" sheetId="1" r:id="rId1"/>
-    <sheet name="Parameters" sheetId="3" r:id="rId2"/>
+    <sheet name="Storage" sheetId="3" r:id="rId2"/>
     <sheet name="Control Map" sheetId="4" r:id="rId3"/>
     <sheet name="Memory" sheetId="2" r:id="rId4"/>
   </sheets>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="117">
   <si>
     <t>USB</t>
   </si>
@@ -335,57 +335,6 @@
     <t>BAT_SENSE</t>
   </si>
   <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Function</t>
-  </si>
-  <si>
-    <t>Motor_PWM_L_MIN</t>
-  </si>
-  <si>
-    <t>minimum PWM value</t>
-  </si>
-  <si>
-    <t>Motor_PWM_L_TRIM</t>
-  </si>
-  <si>
-    <t>Motor_PWM_L_MAX</t>
-  </si>
-  <si>
-    <t>Motor_PWM_L_REVERSED</t>
-  </si>
-  <si>
-    <t>Motor_PWM_L_DZ</t>
-  </si>
-  <si>
-    <t>neutral PWM value</t>
-  </si>
-  <si>
-    <t>max PWM value</t>
-  </si>
-  <si>
-    <t>Deadzone Value</t>
-  </si>
-  <si>
-    <t>PID_POS_X_GAIN_P</t>
-  </si>
-  <si>
-    <t>PID_POS_X_GAIN_I</t>
-  </si>
-  <si>
-    <t>PID_POS_X_GAIN_D</t>
-  </si>
-  <si>
-    <t>BAT_CAPACITY</t>
-  </si>
-  <si>
-    <t>BAT_LOW_LEVEL</t>
-  </si>
-  <si>
-    <t>BAT_CRIT_LEVEL</t>
-  </si>
-  <si>
     <t>y</t>
   </si>
   <si>
@@ -423,6 +372,24 @@
   </si>
   <si>
     <t>y_factor</t>
+  </si>
+  <si>
+    <t>Varriable Name</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Sensor Setting</t>
+  </si>
+  <si>
+    <t>Storage Type</t>
+  </si>
+  <si>
+    <t>NVS</t>
   </si>
 </sst>
 </file>
@@ -994,56 +961,56 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1420,10 +1387,10 @@
       <c r="E1" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="F1" s="59" t="s">
+      <c r="F1" s="55" t="s">
         <v>77</v>
       </c>
-      <c r="G1" s="60"/>
+      <c r="G1" s="56"/>
       <c r="H1" s="13" t="s">
         <v>81</v>
       </c>
@@ -1463,10 +1430,10 @@
       <c r="E3" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="F3" s="51" t="s">
+      <c r="F3" s="57" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="52"/>
+      <c r="G3" s="58"/>
       <c r="H3" s="34">
         <v>23</v>
       </c>
@@ -1495,10 +1462,10 @@
         <v>11</v>
       </c>
       <c r="E4" s="24"/>
-      <c r="F4" s="51" t="s">
+      <c r="F4" s="57" t="s">
         <v>17</v>
       </c>
-      <c r="G4" s="52"/>
+      <c r="G4" s="58"/>
       <c r="H4" s="34">
         <v>22</v>
       </c>
@@ -1528,10 +1495,10 @@
         <v>12</v>
       </c>
       <c r="E5" s="24"/>
-      <c r="F5" s="53" t="s">
+      <c r="F5" s="67" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="54"/>
+      <c r="G5" s="68"/>
       <c r="H5" s="34" t="s">
         <v>5</v>
       </c>
@@ -1559,10 +1526,10 @@
         <v>13</v>
       </c>
       <c r="E6" s="24"/>
-      <c r="F6" s="53" t="s">
+      <c r="F6" s="67" t="s">
         <v>10</v>
       </c>
-      <c r="G6" s="54"/>
+      <c r="G6" s="68"/>
       <c r="H6" s="34" t="s">
         <v>6</v>
       </c>
@@ -1591,10 +1558,10 @@
         <v>14</v>
       </c>
       <c r="E7" s="24"/>
-      <c r="F7" s="51" t="s">
+      <c r="F7" s="57" t="s">
         <v>19</v>
       </c>
-      <c r="G7" s="52"/>
+      <c r="G7" s="58"/>
       <c r="H7" s="34">
         <v>21</v>
       </c>
@@ -1621,8 +1588,8 @@
       </c>
       <c r="D8" s="16"/>
       <c r="E8" s="24"/>
-      <c r="F8" s="55"/>
-      <c r="G8" s="56"/>
+      <c r="F8" s="63"/>
+      <c r="G8" s="64"/>
       <c r="H8" s="35" t="s">
         <v>3</v>
       </c>
@@ -1646,10 +1613,10 @@
       </c>
       <c r="D9" s="16"/>
       <c r="E9" s="24"/>
-      <c r="F9" s="51" t="s">
+      <c r="F9" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="G9" s="52"/>
+      <c r="G9" s="58"/>
       <c r="H9" s="34">
         <v>19</v>
       </c>
@@ -1672,10 +1639,10 @@
         <v>33</v>
       </c>
       <c r="E10" s="24"/>
-      <c r="F10" s="51" t="s">
+      <c r="F10" s="57" t="s">
         <v>21</v>
       </c>
-      <c r="G10" s="52"/>
+      <c r="G10" s="58"/>
       <c r="H10" s="34">
         <v>18</v>
       </c>
@@ -1704,10 +1671,10 @@
         <v>15</v>
       </c>
       <c r="E11" s="24"/>
-      <c r="F11" s="51" t="s">
+      <c r="F11" s="57" t="s">
         <v>22</v>
       </c>
-      <c r="G11" s="52"/>
+      <c r="G11" s="58"/>
       <c r="H11" s="34">
         <v>5</v>
       </c>
@@ -1736,8 +1703,8 @@
         <v>16</v>
       </c>
       <c r="E12" s="24"/>
-      <c r="F12" s="55"/>
-      <c r="G12" s="56"/>
+      <c r="F12" s="63"/>
+      <c r="G12" s="64"/>
       <c r="H12" s="35" t="s">
         <v>3</v>
       </c>
@@ -1760,8 +1727,8 @@
         <v>25</v>
       </c>
       <c r="E13" s="24"/>
-      <c r="F13" s="55"/>
-      <c r="G13" s="56"/>
+      <c r="F13" s="63"/>
+      <c r="G13" s="64"/>
       <c r="H13" s="35" t="s">
         <v>3</v>
       </c>
@@ -1784,10 +1751,10 @@
       <c r="E14" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="F14" s="51" t="s">
+      <c r="F14" s="57" t="s">
         <v>23</v>
       </c>
-      <c r="G14" s="52"/>
+      <c r="G14" s="58"/>
       <c r="H14" s="34">
         <v>4</v>
       </c>
@@ -1814,10 +1781,10 @@
       <c r="E15" s="26" t="s">
         <v>71</v>
       </c>
-      <c r="F15" s="61" t="s">
+      <c r="F15" s="59" t="s">
         <v>73</v>
       </c>
-      <c r="G15" s="62"/>
+      <c r="G15" s="60"/>
       <c r="H15" s="34">
         <v>0</v>
       </c>
@@ -1855,10 +1822,10 @@
       </c>
       <c r="D17" s="16"/>
       <c r="E17" s="24"/>
-      <c r="F17" s="63" t="s">
+      <c r="F17" s="61" t="s">
         <v>26</v>
       </c>
-      <c r="G17" s="64"/>
+      <c r="G17" s="62"/>
       <c r="H17" s="34">
         <v>15</v>
       </c>
@@ -1874,8 +1841,8 @@
       </c>
       <c r="D18" s="16"/>
       <c r="E18" s="24"/>
-      <c r="F18" s="55"/>
-      <c r="G18" s="56"/>
+      <c r="F18" s="63"/>
+      <c r="G18" s="64"/>
       <c r="H18" s="35" t="s">
         <v>3</v>
       </c>
@@ -1892,8 +1859,8 @@
       </c>
       <c r="D19" s="16"/>
       <c r="E19" s="24"/>
-      <c r="F19" s="55"/>
-      <c r="G19" s="56"/>
+      <c r="F19" s="63"/>
+      <c r="G19" s="64"/>
       <c r="H19" s="35" t="s">
         <v>3</v>
       </c>
@@ -1914,8 +1881,8 @@
       <c r="E20" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="F20" s="55"/>
-      <c r="G20" s="56"/>
+      <c r="F20" s="63"/>
+      <c r="G20" s="64"/>
       <c r="H20" s="35" t="s">
         <v>3</v>
       </c>
@@ -1933,8 +1900,8 @@
       <c r="E21" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="F21" s="57"/>
-      <c r="G21" s="58"/>
+      <c r="F21" s="53"/>
+      <c r="G21" s="54"/>
       <c r="H21" s="41" t="s">
         <v>3</v>
       </c>
@@ -2114,6 +2081,10 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="F20:G20"/>
     <mergeCell ref="F21:G21"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="F14:G14"/>
@@ -2130,10 +2101,6 @@
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="F4:G4"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="F20:G20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2141,91 +2108,40 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED2ED9D5-7D28-4E86-BEBD-930593539366}">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33" style="49" customWidth="1"/>
-    <col min="2" max="16384" width="9.140625" style="49"/>
+    <col min="1" max="2" width="13.42578125" style="49" customWidth="1"/>
+    <col min="3" max="3" width="33" style="49" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" style="49" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="49"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="50" t="s">
-        <v>98</v>
+        <v>113</v>
       </c>
       <c r="B1" s="50" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+      <c r="C1" s="50" t="s">
+        <v>111</v>
+      </c>
+      <c r="D1" s="50" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="49" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
       <c r="B2" s="49" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="49" t="s">
-        <v>102</v>
-      </c>
-      <c r="B3" s="49" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="49" t="s">
-        <v>103</v>
-      </c>
-      <c r="B4" s="49" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="49" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="49" t="s">
-        <v>105</v>
-      </c>
-      <c r="B6" s="49" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="49" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="49" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="49" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="49" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="49" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="49" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -2237,14 +2153,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{795C3655-F869-41FB-A905-74C2757B5376}">
   <dimension ref="A1:R22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="4" width="7.42578125" customWidth="1"/>
-    <col min="16" max="18" width="9.140625" style="68"/>
+    <col min="16" max="18" width="9.140625" style="52"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -2252,31 +2168,31 @@
         <v>63</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>115</v>
+        <v>98</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>116</v>
+        <v>99</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>117</v>
+        <v>100</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>118</v>
+        <v>101</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>119</v>
+        <v>102</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="P1" s="67" t="s">
-        <v>124</v>
-      </c>
-      <c r="Q1" s="67" t="s">
-        <v>125</v>
-      </c>
-      <c r="R1" s="67" t="s">
-        <v>126</v>
+        <v>103</v>
+      </c>
+      <c r="P1" s="51" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q1" s="51" t="s">
+        <v>108</v>
+      </c>
+      <c r="R1" s="51" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
@@ -2301,20 +2217,20 @@
         <v>0</v>
       </c>
       <c r="L2" t="s">
-        <v>121</v>
+        <v>104</v>
       </c>
       <c r="M2">
         <v>10000</v>
       </c>
-      <c r="P2" s="68">
+      <c r="P2" s="52">
         <f>G2/$M$2</f>
         <v>0</v>
       </c>
-      <c r="Q2" s="68">
+      <c r="Q2" s="52">
         <f t="shared" ref="Q2:R2" si="0">H2/$M$2</f>
         <v>0</v>
       </c>
-      <c r="R2" s="68">
+      <c r="R2" s="52">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2333,7 +2249,7 @@
         <v>-900</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:H22" si="1">C3*(M$2/M$5)</f>
+        <f t="shared" ref="G3:G22" si="1">C3*(M$2/M$5)</f>
         <v>500</v>
       </c>
       <c r="H3">
@@ -2341,20 +2257,20 @@
         <v>500</v>
       </c>
       <c r="L3" t="s">
-        <v>122</v>
+        <v>105</v>
       </c>
       <c r="M3">
         <v>0</v>
       </c>
-      <c r="P3" s="68">
+      <c r="P3" s="52">
         <f t="shared" ref="P3:P22" si="3">G3/$M$2</f>
         <v>0.05</v>
       </c>
-      <c r="Q3" s="68">
+      <c r="Q3" s="52">
         <f t="shared" ref="Q3:Q22" si="4">H3/$M$2</f>
         <v>0.05</v>
       </c>
-      <c r="R3" s="68">
+      <c r="R3" s="52">
         <f t="shared" ref="R3:R22" si="5">I3/$M$2</f>
         <v>0</v>
       </c>
@@ -2380,15 +2296,15 @@
         <f t="shared" si="2"/>
         <v>1000</v>
       </c>
-      <c r="P4" s="68">
+      <c r="P4" s="52">
         <f t="shared" si="3"/>
         <v>0.1</v>
       </c>
-      <c r="Q4" s="68">
+      <c r="Q4" s="52">
         <f t="shared" si="4"/>
         <v>0.1</v>
       </c>
-      <c r="R4" s="68">
+      <c r="R4" s="52">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -2415,20 +2331,20 @@
         <v>1500</v>
       </c>
       <c r="L5" t="s">
-        <v>123</v>
+        <v>106</v>
       </c>
       <c r="M5">
         <v>1000</v>
       </c>
-      <c r="P5" s="68">
+      <c r="P5" s="52">
         <f t="shared" si="3"/>
         <v>0.15</v>
       </c>
-      <c r="Q5" s="68">
+      <c r="Q5" s="52">
         <f t="shared" si="4"/>
         <v>0.15</v>
       </c>
-      <c r="R5" s="68">
+      <c r="R5" s="52">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -2454,15 +2370,15 @@
         <f t="shared" si="2"/>
         <v>2000</v>
       </c>
-      <c r="P6" s="68">
+      <c r="P6" s="52">
         <f t="shared" si="3"/>
         <v>0.2</v>
       </c>
-      <c r="Q6" s="68">
+      <c r="Q6" s="52">
         <f t="shared" si="4"/>
         <v>0.2</v>
       </c>
-      <c r="R6" s="68">
+      <c r="R6" s="52">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -2488,15 +2404,15 @@
         <f t="shared" si="2"/>
         <v>2500</v>
       </c>
-      <c r="P7" s="68">
+      <c r="P7" s="52">
         <f t="shared" si="3"/>
         <v>0.25</v>
       </c>
-      <c r="Q7" s="68">
+      <c r="Q7" s="52">
         <f t="shared" si="4"/>
         <v>0.25</v>
       </c>
-      <c r="R7" s="68">
+      <c r="R7" s="52">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -2523,20 +2439,20 @@
         <v>3000</v>
       </c>
       <c r="L8" t="s">
-        <v>127</v>
+        <v>110</v>
       </c>
       <c r="M8">
         <v>200</v>
       </c>
-      <c r="P8" s="68">
+      <c r="P8" s="52">
         <f t="shared" si="3"/>
         <v>0.3</v>
       </c>
-      <c r="Q8" s="68">
+      <c r="Q8" s="52">
         <f t="shared" si="4"/>
         <v>0.3</v>
       </c>
-      <c r="R8" s="68">
+      <c r="R8" s="52">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -2562,15 +2478,15 @@
         <f t="shared" si="2"/>
         <v>3500</v>
       </c>
-      <c r="P9" s="68">
+      <c r="P9" s="52">
         <f t="shared" si="3"/>
         <v>0.35</v>
       </c>
-      <c r="Q9" s="68">
+      <c r="Q9" s="52">
         <f t="shared" si="4"/>
         <v>0.35</v>
       </c>
-      <c r="R9" s="68">
+      <c r="R9" s="52">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -2596,15 +2512,15 @@
         <f t="shared" si="2"/>
         <v>4000</v>
       </c>
-      <c r="P10" s="68">
+      <c r="P10" s="52">
         <f t="shared" si="3"/>
         <v>0.4</v>
       </c>
-      <c r="Q10" s="68">
+      <c r="Q10" s="52">
         <f t="shared" si="4"/>
         <v>0.4</v>
       </c>
-      <c r="R10" s="68">
+      <c r="R10" s="52">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -2631,17 +2547,17 @@
         <v>4500</v>
       </c>
       <c r="L11" t="s">
-        <v>115</v>
-      </c>
-      <c r="P11" s="68">
+        <v>98</v>
+      </c>
+      <c r="P11" s="52">
         <f t="shared" si="3"/>
         <v>0.45</v>
       </c>
-      <c r="Q11" s="68">
+      <c r="Q11" s="52">
         <f t="shared" si="4"/>
         <v>0.45</v>
       </c>
-      <c r="R11" s="68">
+      <c r="R11" s="52">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -2667,15 +2583,15 @@
         <f t="shared" si="2"/>
         <v>5000</v>
       </c>
-      <c r="P12" s="68">
+      <c r="P12" s="52">
         <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
-      <c r="Q12" s="68">
+      <c r="Q12" s="52">
         <f t="shared" si="4"/>
         <v>0.5</v>
       </c>
-      <c r="R12" s="68">
+      <c r="R12" s="52">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -2701,15 +2617,15 @@
         <f t="shared" si="2"/>
         <v>5500</v>
       </c>
-      <c r="P13" s="68">
+      <c r="P13" s="52">
         <f t="shared" si="3"/>
         <v>0.55000000000000004</v>
       </c>
-      <c r="Q13" s="68">
+      <c r="Q13" s="52">
         <f t="shared" si="4"/>
         <v>0.55000000000000004</v>
       </c>
-      <c r="R13" s="68">
+      <c r="R13" s="52">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -2735,15 +2651,15 @@
         <f t="shared" si="2"/>
         <v>6000</v>
       </c>
-      <c r="P14" s="68">
+      <c r="P14" s="52">
         <f t="shared" si="3"/>
         <v>0.6</v>
       </c>
-      <c r="Q14" s="68">
+      <c r="Q14" s="52">
         <f t="shared" si="4"/>
         <v>0.6</v>
       </c>
-      <c r="R14" s="68">
+      <c r="R14" s="52">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -2769,15 +2685,15 @@
         <f t="shared" si="2"/>
         <v>6500</v>
       </c>
-      <c r="P15" s="68">
+      <c r="P15" s="52">
         <f t="shared" si="3"/>
         <v>0.65</v>
       </c>
-      <c r="Q15" s="68">
+      <c r="Q15" s="52">
         <f t="shared" si="4"/>
         <v>0.65</v>
       </c>
-      <c r="R15" s="68">
+      <c r="R15" s="52">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -2803,15 +2719,15 @@
         <f t="shared" si="2"/>
         <v>7000</v>
       </c>
-      <c r="P16" s="68">
+      <c r="P16" s="52">
         <f t="shared" si="3"/>
         <v>0.7</v>
       </c>
-      <c r="Q16" s="68">
+      <c r="Q16" s="52">
         <f t="shared" si="4"/>
         <v>0.7</v>
       </c>
-      <c r="R16" s="68">
+      <c r="R16" s="52">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -2837,15 +2753,15 @@
         <f t="shared" si="2"/>
         <v>7500</v>
       </c>
-      <c r="P17" s="68">
+      <c r="P17" s="52">
         <f t="shared" si="3"/>
         <v>0.75</v>
       </c>
-      <c r="Q17" s="68">
+      <c r="Q17" s="52">
         <f t="shared" si="4"/>
         <v>0.75</v>
       </c>
-      <c r="R17" s="68">
+      <c r="R17" s="52">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -2871,15 +2787,15 @@
         <f t="shared" si="2"/>
         <v>8000</v>
       </c>
-      <c r="P18" s="68">
+      <c r="P18" s="52">
         <f t="shared" si="3"/>
         <v>0.8</v>
       </c>
-      <c r="Q18" s="68">
+      <c r="Q18" s="52">
         <f t="shared" si="4"/>
         <v>0.8</v>
       </c>
-      <c r="R18" s="68">
+      <c r="R18" s="52">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -2905,15 +2821,15 @@
         <f t="shared" si="2"/>
         <v>8500</v>
       </c>
-      <c r="P19" s="68">
+      <c r="P19" s="52">
         <f t="shared" si="3"/>
         <v>0.85</v>
       </c>
-      <c r="Q19" s="68">
+      <c r="Q19" s="52">
         <f t="shared" si="4"/>
         <v>0.85</v>
       </c>
-      <c r="R19" s="68">
+      <c r="R19" s="52">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -2939,15 +2855,15 @@
         <f t="shared" si="2"/>
         <v>9000</v>
       </c>
-      <c r="P20" s="68">
+      <c r="P20" s="52">
         <f t="shared" si="3"/>
         <v>0.9</v>
       </c>
-      <c r="Q20" s="68">
+      <c r="Q20" s="52">
         <f t="shared" si="4"/>
         <v>0.9</v>
       </c>
-      <c r="R20" s="68">
+      <c r="R20" s="52">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -2973,15 +2889,15 @@
         <f t="shared" si="2"/>
         <v>9500</v>
       </c>
-      <c r="P21" s="68">
+      <c r="P21" s="52">
         <f t="shared" si="3"/>
         <v>0.95</v>
       </c>
-      <c r="Q21" s="68">
+      <c r="Q21" s="52">
         <f t="shared" si="4"/>
         <v>0.95</v>
       </c>
-      <c r="R21" s="68">
+      <c r="R21" s="52">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -3007,15 +2923,15 @@
         <f t="shared" si="2"/>
         <v>10000</v>
       </c>
-      <c r="P22" s="68">
+      <c r="P22" s="52">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="Q22" s="68">
+      <c r="Q22" s="52">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="R22" s="68">
+      <c r="R22" s="52">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
feat: update sensor system
</commit_message>
<xml_diff>
--- a/firmware/Code/Bicopter_MPU/config_data.xlsx
+++ b/firmware/Code/Bicopter_MPU/config_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\Github\Horizon\firmware\Code\Bicopter_MPU\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{691E5DF0-0280-4AD7-8597-95E81C5E58D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6F2E376-54D6-4D80-BF0A-ECE4F1A0A933}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{2840FDD2-01AF-4896-868F-3F8C8BCC030E}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{2840FDD2-01AF-4896-868F-3F8C8BCC030E}"/>
   </bookViews>
   <sheets>
     <sheet name="Pinout" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="123">
   <si>
     <t>USB</t>
   </si>
@@ -390,6 +390,24 @@
   </si>
   <si>
     <t>NVS</t>
+  </si>
+  <si>
+    <t>SCL</t>
+  </si>
+  <si>
+    <t>SDA</t>
+  </si>
+  <si>
+    <t>Rx_GPS</t>
+  </si>
+  <si>
+    <t>Tx_GPS</t>
+  </si>
+  <si>
+    <t>OutputEN</t>
+  </si>
+  <si>
+    <t>Misc</t>
   </si>
 </sst>
 </file>
@@ -963,6 +981,24 @@
     <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -975,12 +1011,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -993,22 +1023,10 @@
     <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -1353,8 +1371,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D127F088-7B18-4226-A98D-569BDDB3DCA1}">
   <dimension ref="A1:O33"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1387,10 +1405,10 @@
       <c r="E1" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="F1" s="55" t="s">
+      <c r="F1" s="61" t="s">
         <v>77</v>
       </c>
-      <c r="G1" s="56"/>
+      <c r="G1" s="62"/>
       <c r="H1" s="13" t="s">
         <v>81</v>
       </c>
@@ -1406,8 +1424,8 @@
       <c r="E2" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="F2" s="65"/>
-      <c r="G2" s="66"/>
+      <c r="F2" s="67"/>
+      <c r="G2" s="68"/>
       <c r="H2" s="32" t="s">
         <v>3</v>
       </c>
@@ -1430,10 +1448,10 @@
       <c r="E3" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="F3" s="57" t="s">
+      <c r="F3" s="55" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="58"/>
+      <c r="G3" s="56"/>
       <c r="H3" s="34">
         <v>23</v>
       </c>
@@ -1462,10 +1480,10 @@
         <v>11</v>
       </c>
       <c r="E4" s="24"/>
-      <c r="F4" s="57" t="s">
+      <c r="F4" s="55" t="s">
         <v>17</v>
       </c>
-      <c r="G4" s="58"/>
+      <c r="G4" s="56"/>
       <c r="H4" s="34">
         <v>22</v>
       </c>
@@ -1495,15 +1513,15 @@
         <v>12</v>
       </c>
       <c r="E5" s="24"/>
-      <c r="F5" s="67" t="s">
+      <c r="F5" s="53" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="68"/>
+      <c r="G5" s="54"/>
       <c r="H5" s="34" t="s">
         <v>5</v>
       </c>
       <c r="I5" s="43" t="s">
-        <v>62</v>
+        <v>119</v>
       </c>
       <c r="M5" s="1" t="s">
         <v>79</v>
@@ -1526,15 +1544,15 @@
         <v>13</v>
       </c>
       <c r="E6" s="24"/>
-      <c r="F6" s="67" t="s">
+      <c r="F6" s="53" t="s">
         <v>10</v>
       </c>
-      <c r="G6" s="68"/>
+      <c r="G6" s="54"/>
       <c r="H6" s="34" t="s">
         <v>6</v>
       </c>
       <c r="I6" s="44" t="s">
-        <v>95</v>
+        <v>120</v>
       </c>
       <c r="J6" s="9"/>
       <c r="M6" s="1" t="s">
@@ -1558,10 +1576,10 @@
         <v>14</v>
       </c>
       <c r="E7" s="24"/>
-      <c r="F7" s="57" t="s">
+      <c r="F7" s="55" t="s">
         <v>19</v>
       </c>
-      <c r="G7" s="58"/>
+      <c r="G7" s="56"/>
       <c r="H7" s="34">
         <v>21</v>
       </c>
@@ -1581,15 +1599,15 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B8" s="46" t="s">
-        <v>42</v>
+        <v>121</v>
       </c>
       <c r="C8" s="33">
         <v>32</v>
       </c>
       <c r="D8" s="16"/>
       <c r="E8" s="24"/>
-      <c r="F8" s="63"/>
-      <c r="G8" s="64"/>
+      <c r="F8" s="57"/>
+      <c r="G8" s="58"/>
       <c r="H8" s="35" t="s">
         <v>3</v>
       </c>
@@ -1606,17 +1624,17 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B9" s="46" t="s">
-        <v>43</v>
+        <v>122</v>
       </c>
       <c r="C9" s="33">
         <v>33</v>
       </c>
       <c r="D9" s="16"/>
       <c r="E9" s="24"/>
-      <c r="F9" s="57" t="s">
+      <c r="F9" s="55" t="s">
         <v>20</v>
       </c>
-      <c r="G9" s="58"/>
+      <c r="G9" s="56"/>
       <c r="H9" s="34">
         <v>19</v>
       </c>
@@ -1639,10 +1657,10 @@
         <v>33</v>
       </c>
       <c r="E10" s="24"/>
-      <c r="F10" s="57" t="s">
+      <c r="F10" s="55" t="s">
         <v>21</v>
       </c>
-      <c r="G10" s="58"/>
+      <c r="G10" s="56"/>
       <c r="H10" s="34">
         <v>18</v>
       </c>
@@ -1662,7 +1680,7 @@
     </row>
     <row r="11" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="47" t="s">
-        <v>58</v>
+        <v>118</v>
       </c>
       <c r="C11" s="33">
         <v>26</v>
@@ -1671,10 +1689,10 @@
         <v>15</v>
       </c>
       <c r="E11" s="24"/>
-      <c r="F11" s="57" t="s">
+      <c r="F11" s="55" t="s">
         <v>22</v>
       </c>
-      <c r="G11" s="58"/>
+      <c r="G11" s="56"/>
       <c r="H11" s="34">
         <v>5</v>
       </c>
@@ -1694,7 +1712,7 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B12" s="47" t="s">
-        <v>57</v>
+        <v>117</v>
       </c>
       <c r="C12" s="33">
         <v>27</v>
@@ -1703,8 +1721,8 @@
         <v>16</v>
       </c>
       <c r="E12" s="24"/>
-      <c r="F12" s="63"/>
-      <c r="G12" s="64"/>
+      <c r="F12" s="57"/>
+      <c r="G12" s="58"/>
       <c r="H12" s="35" t="s">
         <v>3</v>
       </c>
@@ -1727,8 +1745,8 @@
         <v>25</v>
       </c>
       <c r="E13" s="24"/>
-      <c r="F13" s="63"/>
-      <c r="G13" s="64"/>
+      <c r="F13" s="57"/>
+      <c r="G13" s="58"/>
       <c r="H13" s="35" t="s">
         <v>3</v>
       </c>
@@ -1751,10 +1769,10 @@
       <c r="E14" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="F14" s="57" t="s">
+      <c r="F14" s="55" t="s">
         <v>23</v>
       </c>
-      <c r="G14" s="58"/>
+      <c r="G14" s="56"/>
       <c r="H14" s="34">
         <v>4</v>
       </c>
@@ -1781,10 +1799,10 @@
       <c r="E15" s="26" t="s">
         <v>71</v>
       </c>
-      <c r="F15" s="59" t="s">
+      <c r="F15" s="63" t="s">
         <v>73</v>
       </c>
-      <c r="G15" s="60"/>
+      <c r="G15" s="64"/>
       <c r="H15" s="34">
         <v>0</v>
       </c>
@@ -1822,10 +1840,10 @@
       </c>
       <c r="D17" s="16"/>
       <c r="E17" s="24"/>
-      <c r="F17" s="61" t="s">
+      <c r="F17" s="65" t="s">
         <v>26</v>
       </c>
-      <c r="G17" s="62"/>
+      <c r="G17" s="66"/>
       <c r="H17" s="34">
         <v>15</v>
       </c>
@@ -1841,8 +1859,8 @@
       </c>
       <c r="D18" s="16"/>
       <c r="E18" s="24"/>
-      <c r="F18" s="63"/>
-      <c r="G18" s="64"/>
+      <c r="F18" s="57"/>
+      <c r="G18" s="58"/>
       <c r="H18" s="35" t="s">
         <v>3</v>
       </c>
@@ -1859,8 +1877,8 @@
       </c>
       <c r="D19" s="16"/>
       <c r="E19" s="24"/>
-      <c r="F19" s="63"/>
-      <c r="G19" s="64"/>
+      <c r="F19" s="57"/>
+      <c r="G19" s="58"/>
       <c r="H19" s="35" t="s">
         <v>3</v>
       </c>
@@ -1881,8 +1899,8 @@
       <c r="E20" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="F20" s="63"/>
-      <c r="G20" s="64"/>
+      <c r="F20" s="57"/>
+      <c r="G20" s="58"/>
       <c r="H20" s="35" t="s">
         <v>3</v>
       </c>
@@ -1900,8 +1918,8 @@
       <c r="E21" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="F21" s="53"/>
-      <c r="G21" s="54"/>
+      <c r="F21" s="59"/>
+      <c r="G21" s="60"/>
       <c r="H21" s="41" t="s">
         <v>3</v>
       </c>
@@ -2081,17 +2099,11 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="F21:G21"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="F14:G14"/>
     <mergeCell ref="F15:G15"/>
     <mergeCell ref="F17:G17"/>
     <mergeCell ref="F18:G18"/>
-    <mergeCell ref="F19:G19"/>
     <mergeCell ref="F8:G8"/>
     <mergeCell ref="F9:G9"/>
     <mergeCell ref="F10:G10"/>
@@ -2101,6 +2113,12 @@
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="F4:G4"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="F19:G19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2110,7 +2128,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED2ED9D5-7D28-4E86-BEBD-930593539366}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>

</xml_diff>